<commit_message>
version handed to Helal. runs fine on my computer. -mary
</commit_message>
<xml_diff>
--- a/All_tc_results.xlsx
+++ b/All_tc_results.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test_Case_1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test_Case_2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test_Case_3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test_Case_4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test_Case_5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Test_Case_1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Test_Case_2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Test_Case_3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Test_Case_4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Test_Case_5" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -141,16 +141,16 @@
     <t>Modpath6</t>
   </si>
   <si>
-    <t>9359443.762973258</t>
-  </si>
-  <si>
-    <t>214.8647504665771</t>
+    <t>9359443.762972957</t>
+  </si>
+  <si>
+    <t>214.86475046657017</t>
   </si>
   <si>
     <t>Percent Difference</t>
   </si>
   <si>
-    <t>0.07690028701549567</t>
+    <t>0.07690028701551169</t>
   </si>
   <si>
     <t>9349386.234604424</t>
@@ -837,10 +837,10 @@
         <v>1290.353580075114</v>
       </c>
       <c r="B2" t="n">
-        <v>1279.2661723247</v>
+        <v>1279.268080354399</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8629609684514259</v>
+        <v>0.862811821010453</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -849,19 +849,19 @@
         <v>4053.765327697268</v>
       </c>
       <c r="F2" t="n">
-        <v>3824.3482105084</v>
+        <v>3824.353255349601</v>
       </c>
       <c r="G2" t="n">
-        <v>5.824163769061898</v>
+        <v>5.824031967260432</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
       </c>
       <c r="I2" t="n">
-        <v>-3819.775638094199</v>
+        <v>-3819.780660976099</v>
       </c>
       <c r="J2" t="n">
-        <v>5.943696505033616</v>
+        <v>5.943565124475594</v>
       </c>
       <c r="K2" t="s">
         <v>5</v>
@@ -943,16 +943,16 @@
         <v>41</v>
       </c>
       <c r="D3" t="n">
-        <v>5663596.488198668</v>
+        <v>2333.68519866677</v>
       </c>
       <c r="E3" t="n">
-        <v>19622150.32759855</v>
+        <v>2220.58759854444</v>
       </c>
       <c r="F3" t="n">
-        <v>5667162.882250178</v>
+        <v>5900.079250175982</v>
       </c>
       <c r="G3" t="n">
-        <v>19626018.17588283</v>
+        <v>6088.435882829661</v>
       </c>
     </row>
     <row r="4" spans="1:7">

</xml_diff>

<commit_message>
removed superflouous text from scripts, added dimension pass fail data for tc4 and 5
</commit_message>
<xml_diff>
--- a/All_tc_results.xlsx
+++ b/All_tc_results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>Time_Days</t>
   </si>
@@ -138,6 +138,18 @@
     <t>250.66404873950376</t>
   </si>
   <si>
+    <t>2222.010614165105</t>
+  </si>
+  <si>
+    <t>1952.2631030716002</t>
+  </si>
+  <si>
+    <t>6013.278330701403</t>
+  </si>
+  <si>
+    <t>6507.326095201075</t>
+  </si>
+  <si>
     <t>Modpath6</t>
   </si>
   <si>
@@ -147,10 +159,34 @@
     <t>214.86475046657017</t>
   </si>
   <si>
+    <t>2333.68519866677</t>
+  </si>
+  <si>
+    <t>2220.58759854444</t>
+  </si>
+  <si>
+    <t>5900.079250175981</t>
+  </si>
+  <si>
+    <t>6088.435882829661</t>
+  </si>
+  <si>
     <t>Percent Difference</t>
   </si>
   <si>
-    <t>0.07690028701551169</t>
+    <t>7.690028701551169</t>
+  </si>
+  <si>
+    <t>2.4513178467077372</t>
+  </si>
+  <si>
+    <t>6.430244325993366</t>
+  </si>
+  <si>
+    <t>0.9501862070112219</t>
+  </si>
+  <si>
+    <t>3.325644078556214</t>
   </si>
   <si>
     <t>9349386.234604424</t>
@@ -159,7 +195,31 @@
     <t>214.63385978781378</t>
   </si>
   <si>
-    <t>0.07743466775023054</t>
+    <t>2332.568630426191</t>
+  </si>
+  <si>
+    <t>2061.142585285008</t>
+  </si>
+  <si>
+    <t>5900.046642815694</t>
+  </si>
+  <si>
+    <t>5929.750451251864</t>
+  </si>
+  <si>
+    <t>7.743466775023054</t>
+  </si>
+  <si>
+    <t>2.4274035058754757</t>
+  </si>
+  <si>
+    <t>2.712894999109628</t>
+  </si>
+  <si>
+    <t>0.9504625126689582</t>
+  </si>
+  <si>
+    <t>4.6439823843806405</t>
   </si>
 </sst>
 </file>
@@ -919,56 +979,64 @@
       <c r="C2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" t="n">
-        <v>5663484.813779525</v>
-      </c>
-      <c r="E2" t="n">
-        <v>19622042.00749284</v>
-      </c>
-      <c r="F2" t="n">
-        <v>5667276.081496061</v>
-      </c>
-      <c r="G2" t="n">
-        <v>19626597.07048497</v>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2333.68519866677</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2220.58759854444</v>
-      </c>
-      <c r="F3" t="n">
-        <v>5900.079250175982</v>
-      </c>
-      <c r="G3" t="n">
-        <v>6088.435882829661</v>
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s"/>
-      <c r="E4" t="s"/>
-      <c r="F4" t="s"/>
-      <c r="G4" t="s"/>
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
@@ -980,10 +1048,18 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s"/>
-      <c r="E5" t="s"/>
-      <c r="F5" t="s"/>
-      <c r="G5" t="s"/>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1037,56 +1113,64 @@
       <c r="C2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" t="n">
-        <v>5663484.813779525</v>
-      </c>
-      <c r="E2" t="n">
-        <v>19622042.00749284</v>
-      </c>
-      <c r="F2" t="n">
-        <v>5667276.081496061</v>
-      </c>
-      <c r="G2" t="n">
-        <v>19626597.07048497</v>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" t="n">
-        <v>5663595.371795787</v>
-      </c>
-      <c r="E3" t="n">
-        <v>19622150.88697505</v>
-      </c>
-      <c r="F3" t="n">
-        <v>5667162.849808175</v>
-      </c>
-      <c r="G3" t="n">
-        <v>19626019.49484102</v>
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" t="s"/>
-      <c r="E4" t="s"/>
-      <c r="F4" t="s"/>
-      <c r="G4" t="s"/>
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
@@ -1098,10 +1182,18 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s"/>
-      <c r="E5" t="s"/>
-      <c r="F5" t="s"/>
-      <c r="G5" t="s"/>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
tests and document as passed off to Greg
</commit_message>
<xml_diff>
--- a/All_tc_results.xlsx
+++ b/All_tc_results.xlsx
@@ -153,73 +153,73 @@
     <t>Modpath6</t>
   </si>
   <si>
-    <t>9359443.762972957</t>
-  </si>
-  <si>
-    <t>214.86475046657017</t>
-  </si>
-  <si>
-    <t>2333.68519866677</t>
-  </si>
-  <si>
-    <t>2220.58759854444</t>
-  </si>
-  <si>
-    <t>5900.079250175981</t>
-  </si>
-  <si>
-    <t>6088.435882829661</t>
+    <t>9354317.212192766</t>
+  </si>
+  <si>
+    <t>214.74706024030934</t>
+  </si>
+  <si>
+    <t>2355.3772450506603</t>
+  </si>
+  <si>
+    <t>2197.4601353337093</t>
+  </si>
+  <si>
+    <t>5941.83402009447</t>
+  </si>
+  <si>
+    <t>5976.18170204034</t>
   </si>
   <si>
     <t>Percent Difference</t>
   </si>
   <si>
-    <t>7.690028701551169</t>
-  </si>
-  <si>
-    <t>2.4513178467077372</t>
-  </si>
-  <si>
-    <t>6.430244325993366</t>
-  </si>
-  <si>
-    <t>0.9501862070112219</t>
-  </si>
-  <si>
-    <t>3.325644078556214</t>
-  </si>
-  <si>
-    <t>9349386.234604424</t>
-  </si>
-  <si>
-    <t>214.63385978781378</t>
-  </si>
-  <si>
-    <t>2332.568630426191</t>
-  </si>
-  <si>
-    <t>2061.142585285008</t>
-  </si>
-  <si>
-    <t>5900.046642815694</t>
-  </si>
-  <si>
-    <t>5929.750451251864</t>
-  </si>
-  <si>
-    <t>7.743466775023054</t>
-  </si>
-  <si>
-    <t>2.4274035058754757</t>
-  </si>
-  <si>
-    <t>2.712894999109628</t>
-  </si>
-  <si>
-    <t>0.9504625126689582</t>
-  </si>
-  <si>
-    <t>4.6439823843806405</t>
+    <t>7.71726067689379</t>
+  </si>
+  <si>
+    <t>2.9135969025881248</t>
+  </si>
+  <si>
+    <t>5.908756275426588</t>
+  </si>
+  <si>
+    <t>0.5976046774849153</t>
+  </si>
+  <si>
+    <t>4.254768786046714</t>
+  </si>
+  <si>
+    <t>9367480.367901502</t>
+  </si>
+  <si>
+    <t>215.0492468059148</t>
+  </si>
+  <si>
+    <t>2354.5218369839713</t>
+  </si>
+  <si>
+    <t>2038.3388591967523</t>
+  </si>
+  <si>
+    <t>5941.090629167855</t>
+  </si>
+  <si>
+    <t>5817.6381606943905</t>
+  </si>
+  <si>
+    <t>7.647366367730347</t>
+  </si>
+  <si>
+    <t>2.8954503050796774</t>
+  </si>
+  <si>
+    <t>2.156961705001133</t>
+  </si>
+  <si>
+    <t>0.6038604110002143</t>
+  </si>
+  <si>
+    <t>5.595861539126026</t>
   </si>
 </sst>
 </file>
@@ -897,10 +897,10 @@
         <v>1290.353580075114</v>
       </c>
       <c r="B2" t="n">
-        <v>1279.268080354399</v>
+        <v>1282.669543993601</v>
       </c>
       <c r="C2" t="n">
-        <v>0.862811821010453</v>
+        <v>0.5972768771205283</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -909,19 +909,19 @@
         <v>4053.765327697268</v>
       </c>
       <c r="F2" t="n">
-        <v>3824.353255349601</v>
+        <v>3832.8930403376</v>
       </c>
       <c r="G2" t="n">
-        <v>5.824031967260432</v>
+        <v>5.601162800581742</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
       </c>
       <c r="I2" t="n">
-        <v>-3819.780660976099</v>
+        <v>-3828.310450015801</v>
       </c>
       <c r="J2" t="n">
-        <v>5.943565124475594</v>
+        <v>5.720698050606194</v>
       </c>
       <c r="K2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Final push, minor edits made to scripts during writeup
</commit_message>
<xml_diff>
--- a/All_tc_results.xlsx
+++ b/All_tc_results.xlsx
@@ -598,13 +598,13 @@
         <v>2500</v>
       </c>
       <c r="B2" t="n">
-        <v>2072.753715666667</v>
+        <v>2071.1659551</v>
       </c>
       <c r="C2" t="n">
         <v>2071.040116692083</v>
       </c>
       <c r="D2" t="n">
-        <v>0.05513024589113813</v>
+        <v>0.004050567304590923</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -615,13 +615,13 @@
         <v>5000</v>
       </c>
       <c r="B3" t="n">
-        <v>2920.183220916666</v>
+        <v>2916.6421686</v>
       </c>
       <c r="C3" t="n">
         <v>2921.260914261809</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.02460030086518687</v>
+        <v>-0.1055165180861513</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -632,13 +632,13 @@
         <v>7500</v>
       </c>
       <c r="B4" t="n">
-        <v>3575.155671333333</v>
+        <v>3574.7105138</v>
       </c>
       <c r="C4" t="n">
         <v>3574.768796944108</v>
       </c>
       <c r="D4" t="n">
-        <v>0.007214386917194273</v>
+        <v>-0.001086947267102302</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>

</xml_diff>